<commit_message>
add download template service
</commit_message>
<xml_diff>
--- a/template-BE/reports/ltb/1000455_Togle clamp patah/Togle clamp patah.xlsx
+++ b/template-BE/reports/ltb/1000455_Togle clamp patah/Togle clamp patah.xlsx
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="127">
   <si>
     <r>
       <rPr>
@@ -376,9 +376,6 @@
   </si>
   <si>
     <t>8. ITEM YANG PERLU DILAKUKAN / NEXT ACTION</t>
-  </si>
-  <si>
-    <t>O</t>
   </si>
   <si>
     <t>Items</t>
@@ -7208,9 +7205,7 @@
       <c r="I35" s="116"/>
       <c r="J35" s="116"/>
       <c r="K35" s="117"/>
-      <c r="L35" s="258" t="s">
-        <v>83</v>
-      </c>
+      <c r="L35" s="258"/>
       <c r="M35" s="258"/>
       <c r="N35" s="258"/>
       <c r="O35" s="258"/>
@@ -7250,9 +7245,7 @@
       <c r="AW35" s="253"/>
       <c r="AX35" s="253"/>
       <c r="AY35" s="253"/>
-      <c r="AZ35" s="253" t="s">
-        <v>83</v>
-      </c>
+      <c r="AZ35" s="253"/>
       <c r="BA35" s="253"/>
       <c r="BB35" s="253"/>
       <c r="BC35" s="253"/>
@@ -7321,7 +7314,7 @@
       <c r="DN35" s="18"/>
       <c r="DZ35" s="259"/>
       <c r="EA35" s="260" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="EB35" s="261"/>
       <c r="EC35" s="261"/>
@@ -7337,18 +7330,18 @@
       <c r="EK35" s="261"/>
       <c r="EL35" s="262"/>
       <c r="EM35" s="260" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="EN35" s="262"/>
       <c r="EO35" s="263" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" ht="18" customHeight="1" spans="2:145" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="264"/>
       <c r="E36" s="265" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F36" s="266"/>
       <c r="G36" s="266"/>
@@ -7357,7 +7350,7 @@
       <c r="J36" s="266"/>
       <c r="K36" s="267"/>
       <c r="M36" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N36" s="268"/>
       <c r="O36" s="268"/>
@@ -7369,7 +7362,7 @@
       <c r="U36" s="268"/>
       <c r="V36" s="269"/>
       <c r="W36" s="242" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="X36" s="243"/>
       <c r="Y36" s="243"/>
@@ -7387,7 +7380,7 @@
       <c r="AK36" s="270"/>
       <c r="AL36" s="270"/>
       <c r="AM36" s="271" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AN36" s="271"/>
       <c r="AO36" s="271"/>
@@ -7420,7 +7413,7 @@
       <c r="BP36" s="271"/>
       <c r="BQ36" s="272"/>
       <c r="BR36" s="273" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="BS36" s="273"/>
       <c r="BT36" s="273"/>
@@ -7472,7 +7465,7 @@
       <c r="DN36" s="18"/>
       <c r="DZ36" s="275"/>
       <c r="EA36" s="276" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="EB36" s="277"/>
       <c r="EC36" s="277"/>
@@ -7514,7 +7507,7 @@
       <c r="Y37" s="289"/>
       <c r="Z37" s="289"/>
       <c r="AA37" s="290" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB37" s="289"/>
       <c r="AC37" s="289"/>
@@ -7609,7 +7602,7 @@
       <c r="DN37" s="18"/>
       <c r="DZ37" s="295"/>
       <c r="EA37" s="296" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="EB37" s="297"/>
       <c r="EC37" s="298"/>
@@ -7630,7 +7623,7 @@
       <c r="B38" s="5"/>
       <c r="C38" s="264"/>
       <c r="H38" s="290" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M38" s="285"/>
       <c r="N38" s="286"/>
@@ -7643,7 +7636,7 @@
       <c r="U38" s="286"/>
       <c r="V38" s="287"/>
       <c r="W38" s="242" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X38" s="243"/>
       <c r="Y38" s="243"/>
@@ -7742,7 +7735,7 @@
       <c r="DN38" s="18"/>
       <c r="DZ38" s="304"/>
       <c r="EA38" s="296" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="EB38" s="298"/>
       <c r="EC38" s="298"/>
@@ -7763,7 +7756,7 @@
       <c r="B39" s="5"/>
       <c r="C39" s="264"/>
       <c r="E39" s="265" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F39" s="266"/>
       <c r="G39" s="266"/>
@@ -7786,7 +7779,7 @@
       <c r="Y39" s="289"/>
       <c r="Z39" s="289"/>
       <c r="AA39" s="290" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB39" s="289"/>
       <c r="AC39" s="289"/>
@@ -7881,7 +7874,7 @@
       <c r="DN39" s="18"/>
       <c r="DZ39" s="295"/>
       <c r="EA39" s="296" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="EB39" s="297"/>
       <c r="EC39" s="298"/>
@@ -8016,7 +8009,7 @@
       <c r="DN40" s="18"/>
       <c r="DZ40" s="306"/>
       <c r="EA40" s="307" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="EB40" s="308"/>
       <c r="EC40" s="309"/>
@@ -8037,7 +8030,7 @@
       <c r="B41" s="5"/>
       <c r="C41" s="264"/>
       <c r="H41" s="290" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M41" s="285"/>
       <c r="N41" s="286"/>
@@ -8054,7 +8047,7 @@
       <c r="Y41" s="314"/>
       <c r="Z41" s="314"/>
       <c r="AA41" s="290" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB41" s="314"/>
       <c r="AC41" s="314"/>
@@ -8152,7 +8145,7 @@
       <c r="B42" s="5"/>
       <c r="C42" s="264"/>
       <c r="E42" s="265" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F42" s="266"/>
       <c r="G42" s="266"/>
@@ -8292,7 +8285,7 @@
       <c r="Y43" s="314"/>
       <c r="Z43" s="314"/>
       <c r="AA43" s="290" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB43" s="314"/>
       <c r="AC43" s="314"/>
@@ -8390,7 +8383,7 @@
       <c r="B44" s="5"/>
       <c r="C44" s="264"/>
       <c r="H44" s="290" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M44" s="285"/>
       <c r="N44" s="286"/>
@@ -8503,7 +8496,7 @@
       <c r="B45" s="5"/>
       <c r="C45" s="264"/>
       <c r="E45" s="265" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F45" s="266"/>
       <c r="G45" s="266"/>
@@ -8522,14 +8515,14 @@
       <c r="U45" s="286"/>
       <c r="V45" s="287"/>
       <c r="W45" s="320" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X45" s="321"/>
       <c r="Y45" s="321"/>
       <c r="Z45" s="321"/>
       <c r="AA45" s="321"/>
       <c r="AB45" s="322" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AC45" s="321"/>
       <c r="AD45" s="321"/>
@@ -8585,7 +8578,7 @@
       <c r="CB45" s="324"/>
       <c r="CC45" s="200"/>
       <c r="CD45" s="325" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="CE45" s="326"/>
       <c r="CF45" s="326"/>
@@ -8645,7 +8638,7 @@
       <c r="U46" s="286"/>
       <c r="V46" s="287"/>
       <c r="W46" s="329" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="X46" s="15" t="s">
         <v>14</v>
@@ -8664,7 +8657,7 @@
       <c r="AJ46" s="16"/>
       <c r="AK46" s="17"/>
       <c r="AL46" s="330" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AM46" s="331"/>
       <c r="AN46" s="331"/>
@@ -8699,7 +8692,7 @@
       <c r="BM46" s="335"/>
       <c r="BN46" s="336"/>
       <c r="BO46" s="330" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="BP46" s="331"/>
       <c r="BQ46" s="331"/>
@@ -8710,7 +8703,7 @@
       <c r="BV46" s="331"/>
       <c r="BW46" s="332"/>
       <c r="BX46" s="330" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BY46" s="331"/>
       <c r="BZ46" s="331"/>
@@ -8750,7 +8743,7 @@
       <c r="DB46" s="165"/>
       <c r="DC46" s="165"/>
       <c r="DD46" s="165" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="DE46" s="165"/>
       <c r="DF46" s="165"/>
@@ -8758,7 +8751,7 @@
       <c r="DH46" s="165"/>
       <c r="DI46" s="165"/>
       <c r="DJ46" s="337" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="DK46" s="338"/>
       <c r="DL46" s="338"/>
@@ -8769,7 +8762,7 @@
       <c r="B47" s="5"/>
       <c r="C47" s="264"/>
       <c r="H47" s="290" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M47" s="285"/>
       <c r="N47" s="286"/>
@@ -8882,7 +8875,7 @@
       <c r="B48" s="5"/>
       <c r="C48" s="264"/>
       <c r="E48" s="351" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F48" s="352"/>
       <c r="G48" s="352"/>
@@ -9355,7 +9348,7 @@
     <row r="52" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" ht="15.6" customHeight="1" spans="3:118" x14ac:dyDescent="0.25">
       <c r="C55" s="107" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D55" s="107"/>
       <c r="E55" s="107"/>
@@ -9377,7 +9370,7 @@
       <c r="U55" s="386"/>
       <c r="V55" s="386"/>
       <c r="W55" s="107" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X55" s="107"/>
       <c r="Y55" s="107"/>
@@ -9480,7 +9473,7 @@
         <v>75</v>
       </c>
       <c r="D56" s="388" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E56" s="389"/>
       <c r="F56" s="389"/>
@@ -9504,7 +9497,7 @@
         <v>57</v>
       </c>
       <c r="X56" s="388" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Y56" s="389"/>
       <c r="Z56" s="389"/>
@@ -9512,7 +9505,7 @@
       <c r="AB56" s="389"/>
       <c r="AC56" s="389"/>
       <c r="AD56" s="341" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AE56" s="390"/>
       <c r="AF56" s="390"/>
@@ -9608,7 +9601,7 @@
         <v>76</v>
       </c>
       <c r="D57" s="388" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E57" s="389"/>
       <c r="F57" s="389"/>
@@ -9632,7 +9625,7 @@
         <v>60</v>
       </c>
       <c r="X57" s="388" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y57" s="389"/>
       <c r="Z57" s="389"/>
@@ -9640,7 +9633,7 @@
       <c r="AB57" s="389"/>
       <c r="AC57" s="389"/>
       <c r="AD57" s="341" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE57" s="390"/>
       <c r="AF57" s="390"/>
@@ -9736,7 +9729,7 @@
         <v>77</v>
       </c>
       <c r="D58" s="388" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E58" s="389"/>
       <c r="F58" s="389"/>
@@ -9760,7 +9753,7 @@
         <v>61</v>
       </c>
       <c r="X58" s="388" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Y58" s="389"/>
       <c r="Z58" s="389"/>
@@ -9768,7 +9761,7 @@
       <c r="AB58" s="389"/>
       <c r="AC58" s="389"/>
       <c r="AD58" s="341" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AE58" s="390"/>
       <c r="AF58" s="390"/>
@@ -9864,7 +9857,7 @@
         <v>78</v>
       </c>
       <c r="D59" s="388" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E59" s="389"/>
       <c r="F59" s="389"/>
@@ -9888,7 +9881,7 @@
         <v>63</v>
       </c>
       <c r="X59" s="388" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Y59" s="389"/>
       <c r="Z59" s="389"/>
@@ -9896,7 +9889,7 @@
       <c r="AB59" s="389"/>
       <c r="AC59" s="389"/>
       <c r="AD59" s="341" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AE59" s="390"/>
       <c r="AF59" s="390"/>
@@ -9992,7 +9985,7 @@
         <v>79</v>
       </c>
       <c r="D60" s="388" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E60" s="389"/>
       <c r="F60" s="389"/>
@@ -10016,7 +10009,7 @@
         <v>66</v>
       </c>
       <c r="X60" s="388" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Y60" s="389"/>
       <c r="Z60" s="389"/>
@@ -10024,7 +10017,7 @@
       <c r="AB60" s="389"/>
       <c r="AC60" s="389"/>
       <c r="AD60" s="341" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE60" s="390"/>
       <c r="AF60" s="390"/>
@@ -10120,7 +10113,7 @@
         <v>80</v>
       </c>
       <c r="D61" s="388" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E61" s="389"/>
       <c r="F61" s="389"/>
@@ -10144,7 +10137,7 @@
         <v>68</v>
       </c>
       <c r="X61" s="388" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Y61" s="389"/>
       <c r="Z61" s="389"/>
@@ -10152,7 +10145,7 @@
       <c r="AB61" s="389"/>
       <c r="AC61" s="389"/>
       <c r="AD61" s="341" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE61" s="390"/>
       <c r="AF61" s="390"/>

</xml_diff>